<commit_message>
flexible writing in excel
</commit_message>
<xml_diff>
--- a/DataAgregation/age-clusters.xlsx
+++ b/DataAgregation/age-clusters.xlsx
@@ -5,28 +5,28 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="DAU" sheetId="12" r:id="rId18"/>
-    <sheet name="New Users" sheetId="13" r:id="rId20"/>
-    <sheet name="Revenue" sheetId="14" r:id="rId21"/>
-    <sheet name="MAU" sheetId="15" r:id="rId22"/>
+    <sheet name="DAU" sheetId="24" r:id="rId33"/>
+    <sheet name="New Users" sheetId="25" r:id="rId35"/>
+    <sheet name="Revenue" sheetId="26" r:id="rId36"/>
+    <sheet name="MAU" sheetId="27" r:id="rId38"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>13-25</t>
-  </si>
-  <si>
-    <t>26-39</t>
-  </si>
-  <si>
-    <t>40-52</t>
+    <t>13-24</t>
+  </si>
+  <si>
+    <t>25-38</t>
+  </si>
+  <si>
+    <t>39-52</t>
   </si>
   <si>
     <t>53-64</t>
@@ -120,18 +120,6 @@
   </si>
   <si>
     <t>30.01.2018</t>
-  </si>
-  <si>
-    <t>13-23</t>
-  </si>
-  <si>
-    <t>24-36</t>
-  </si>
-  <si>
-    <t>37-49</t>
-  </si>
-  <si>
-    <t>50-64</t>
   </si>
   <si>
     <t>13-26</t>
@@ -187,7 +175,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -200,16 +188,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -727,7 +715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -740,16 +728,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -1267,7 +1255,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -1280,16 +1268,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -1297,16 +1285,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="0">
-        <v>2118</v>
+        <v>1814</v>
       </c>
       <c r="C2" s="0">
-        <v>1943</v>
+        <v>1988</v>
       </c>
       <c r="D2" s="0">
-        <v>2216</v>
+        <v>2217</v>
       </c>
       <c r="E2" s="0">
-        <v>1881</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="3">
@@ -1314,16 +1302,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="0">
-        <v>4495</v>
+        <v>3858</v>
       </c>
       <c r="C3" s="0">
-        <v>4532</v>
+        <v>4634</v>
       </c>
       <c r="D3" s="0">
-        <v>4356</v>
+        <v>4614</v>
       </c>
       <c r="E3" s="0">
-        <v>3076</v>
+        <v>3353</v>
       </c>
     </row>
     <row r="4">
@@ -1331,16 +1319,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="0">
-        <v>6527</v>
+        <v>5371</v>
       </c>
       <c r="C4" s="0">
-        <v>5868</v>
+        <v>6149</v>
       </c>
       <c r="D4" s="0">
-        <v>5723</v>
+        <v>6108</v>
       </c>
       <c r="E4" s="0">
-        <v>4733</v>
+        <v>5223</v>
       </c>
     </row>
     <row r="5">
@@ -1348,16 +1336,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="0">
-        <v>8778</v>
+        <v>8003</v>
       </c>
       <c r="C5" s="0">
-        <v>8398</v>
+        <v>8159</v>
       </c>
       <c r="D5" s="0">
-        <v>7611</v>
+        <v>8068</v>
       </c>
       <c r="E5" s="0">
-        <v>7499</v>
+        <v>8056</v>
       </c>
     </row>
     <row r="6">
@@ -1365,16 +1353,16 @@
         <v>9</v>
       </c>
       <c r="B6" s="0">
-        <v>11043</v>
+        <v>9475</v>
       </c>
       <c r="C6" s="0">
-        <v>11234</v>
+        <v>11190</v>
       </c>
       <c r="D6" s="0">
-        <v>9578</v>
+        <v>10526</v>
       </c>
       <c r="E6" s="0">
-        <v>8472</v>
+        <v>9136</v>
       </c>
     </row>
     <row r="7">
@@ -1382,16 +1370,16 @@
         <v>10</v>
       </c>
       <c r="B7" s="0">
-        <v>13307</v>
+        <v>11365</v>
       </c>
       <c r="C7" s="0">
-        <v>13544</v>
+        <v>14003</v>
       </c>
       <c r="D7" s="0">
-        <v>11224</v>
+        <v>11535</v>
       </c>
       <c r="E7" s="0">
-        <v>10583</v>
+        <v>11755</v>
       </c>
     </row>
     <row r="8">
@@ -1399,16 +1387,16 @@
         <v>11</v>
       </c>
       <c r="B8" s="0">
-        <v>13338</v>
+        <v>11545</v>
       </c>
       <c r="C8" s="0">
-        <v>13505</v>
+        <v>13527</v>
       </c>
       <c r="D8" s="0">
-        <v>13831</v>
+        <v>14331</v>
       </c>
       <c r="E8" s="0">
-        <v>11770</v>
+        <v>13041</v>
       </c>
     </row>
     <row r="9">
@@ -1416,16 +1404,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="0">
-        <v>15853</v>
+        <v>13874</v>
       </c>
       <c r="C9" s="0">
-        <v>17897</v>
+        <v>17162</v>
       </c>
       <c r="D9" s="0">
-        <v>16121</v>
+        <v>17332</v>
       </c>
       <c r="E9" s="0">
-        <v>13934</v>
+        <v>15437</v>
       </c>
     </row>
     <row r="10">
@@ -1433,16 +1421,16 @@
         <v>13</v>
       </c>
       <c r="B10" s="0">
-        <v>19619</v>
+        <v>16245</v>
       </c>
       <c r="C10" s="0">
-        <v>18877</v>
+        <v>19649</v>
       </c>
       <c r="D10" s="0">
-        <v>17476</v>
+        <v>19033</v>
       </c>
       <c r="E10" s="0">
-        <v>13671</v>
+        <v>14716</v>
       </c>
     </row>
     <row r="11">
@@ -1450,16 +1438,16 @@
         <v>14</v>
       </c>
       <c r="B11" s="0">
-        <v>22748</v>
+        <v>19136</v>
       </c>
       <c r="C11" s="0">
-        <v>20317</v>
+        <v>20676</v>
       </c>
       <c r="D11" s="0">
-        <v>19229</v>
+        <v>21334</v>
       </c>
       <c r="E11" s="0">
-        <v>16105</v>
+        <v>17253</v>
       </c>
     </row>
     <row r="12">
@@ -1467,16 +1455,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="0">
-        <v>24957</v>
+        <v>21625</v>
       </c>
       <c r="C12" s="0">
-        <v>23094</v>
+        <v>23426</v>
       </c>
       <c r="D12" s="0">
-        <v>21767</v>
+        <v>22869</v>
       </c>
       <c r="E12" s="0">
-        <v>19755</v>
+        <v>21653</v>
       </c>
     </row>
     <row r="13">
@@ -1484,16 +1472,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="0">
-        <v>26175</v>
+        <v>22608</v>
       </c>
       <c r="C13" s="0">
-        <v>26387</v>
+        <v>26218</v>
       </c>
       <c r="D13" s="0">
-        <v>22719</v>
+        <v>25077</v>
       </c>
       <c r="E13" s="0">
-        <v>19974</v>
+        <v>21352</v>
       </c>
     </row>
     <row r="14">
@@ -1501,16 +1489,16 @@
         <v>17</v>
       </c>
       <c r="B14" s="0">
-        <v>26465</v>
+        <v>22981</v>
       </c>
       <c r="C14" s="0">
-        <v>26229</v>
+        <v>25777</v>
       </c>
       <c r="D14" s="0">
-        <v>25928</v>
+        <v>27485</v>
       </c>
       <c r="E14" s="0">
-        <v>21349</v>
+        <v>23728</v>
       </c>
     </row>
     <row r="15">
@@ -1518,16 +1506,16 @@
         <v>18</v>
       </c>
       <c r="B15" s="0">
-        <v>28989</v>
+        <v>24850</v>
       </c>
       <c r="C15" s="0">
-        <v>28434</v>
+        <v>28469</v>
       </c>
       <c r="D15" s="0">
-        <v>28085</v>
+        <v>29964</v>
       </c>
       <c r="E15" s="0">
-        <v>24253</v>
+        <v>26478</v>
       </c>
     </row>
     <row r="16">
@@ -1535,16 +1523,16 @@
         <v>19</v>
       </c>
       <c r="B16" s="0">
-        <v>32510</v>
+        <v>27991</v>
       </c>
       <c r="C16" s="0">
-        <v>30790</v>
+        <v>30257</v>
       </c>
       <c r="D16" s="0">
-        <v>28335</v>
+        <v>31238</v>
       </c>
       <c r="E16" s="0">
-        <v>24873</v>
+        <v>27022</v>
       </c>
     </row>
     <row r="17">
@@ -1552,16 +1540,16 @@
         <v>20</v>
       </c>
       <c r="B17" s="0">
-        <v>32601</v>
+        <v>28260</v>
       </c>
       <c r="C17" s="0">
-        <v>33116</v>
+        <v>32795</v>
       </c>
       <c r="D17" s="0">
-        <v>31450</v>
+        <v>34141</v>
       </c>
       <c r="E17" s="0">
-        <v>27377</v>
+        <v>29348</v>
       </c>
     </row>
     <row r="18">
@@ -1569,16 +1557,16 @@
         <v>21</v>
       </c>
       <c r="B18" s="0">
-        <v>38339</v>
+        <v>33646</v>
       </c>
       <c r="C18" s="0">
-        <v>35270</v>
+        <v>35554</v>
       </c>
       <c r="D18" s="0">
-        <v>36335</v>
+        <v>37675</v>
       </c>
       <c r="E18" s="0">
-        <v>26653</v>
+        <v>29722</v>
       </c>
     </row>
     <row r="19">
@@ -1586,16 +1574,16 @@
         <v>22</v>
       </c>
       <c r="B19" s="0">
-        <v>39719</v>
+        <v>34595</v>
       </c>
       <c r="C19" s="0">
-        <v>40964</v>
+        <v>40595</v>
       </c>
       <c r="D19" s="0">
-        <v>34013</v>
+        <v>37125</v>
       </c>
       <c r="E19" s="0">
-        <v>30563</v>
+        <v>32944</v>
       </c>
     </row>
     <row r="20">
@@ -1603,16 +1591,16 @@
         <v>23</v>
       </c>
       <c r="B20" s="0">
-        <v>39273</v>
+        <v>34141</v>
       </c>
       <c r="C20" s="0">
-        <v>41373</v>
+        <v>40661</v>
       </c>
       <c r="D20" s="0">
-        <v>39036</v>
+        <v>42326</v>
       </c>
       <c r="E20" s="0">
-        <v>33594</v>
+        <v>36148</v>
       </c>
     </row>
     <row r="21">
@@ -1620,16 +1608,16 @@
         <v>24</v>
       </c>
       <c r="B21" s="0">
-        <v>42909</v>
+        <v>36586</v>
       </c>
       <c r="C21" s="0">
-        <v>43715</v>
+        <v>44057</v>
       </c>
       <c r="D21" s="0">
-        <v>39681</v>
+        <v>42470</v>
       </c>
       <c r="E21" s="0">
-        <v>34100</v>
+        <v>37292</v>
       </c>
     </row>
     <row r="22">
@@ -1637,16 +1625,16 @@
         <v>25</v>
       </c>
       <c r="B22" s="0">
-        <v>47191</v>
+        <v>40775</v>
       </c>
       <c r="C22" s="0">
-        <v>46144</v>
+        <v>45303</v>
       </c>
       <c r="D22" s="0">
-        <v>40408</v>
+        <v>44598</v>
       </c>
       <c r="E22" s="0">
-        <v>35009</v>
+        <v>38076</v>
       </c>
     </row>
     <row r="23">
@@ -1654,16 +1642,16 @@
         <v>26</v>
       </c>
       <c r="B23" s="0">
-        <v>46877</v>
+        <v>40885</v>
       </c>
       <c r="C23" s="0">
-        <v>45965</v>
+        <v>44304</v>
       </c>
       <c r="D23" s="0">
-        <v>44314</v>
+        <v>49117</v>
       </c>
       <c r="E23" s="0">
-        <v>37973</v>
+        <v>40823</v>
       </c>
     </row>
     <row r="24">
@@ -1671,16 +1659,16 @@
         <v>27</v>
       </c>
       <c r="B24" s="0">
-        <v>48386</v>
+        <v>41177</v>
       </c>
       <c r="C24" s="0">
-        <v>49705</v>
+        <v>50020</v>
       </c>
       <c r="D24" s="0">
-        <v>43470</v>
+        <v>46553</v>
       </c>
       <c r="E24" s="0">
-        <v>38917</v>
+        <v>42728</v>
       </c>
     </row>
     <row r="25">
@@ -1688,16 +1676,16 @@
         <v>28</v>
       </c>
       <c r="B25" s="0">
-        <v>52119</v>
+        <v>45135</v>
       </c>
       <c r="C25" s="0">
-        <v>51968</v>
+        <v>51127</v>
       </c>
       <c r="D25" s="0">
-        <v>48816</v>
+        <v>53057</v>
       </c>
       <c r="E25" s="0">
-        <v>40643</v>
+        <v>44227</v>
       </c>
     </row>
     <row r="26">
@@ -1705,16 +1693,16 @@
         <v>29</v>
       </c>
       <c r="B26" s="0">
-        <v>52163</v>
+        <v>45115</v>
       </c>
       <c r="C26" s="0">
-        <v>54169</v>
+        <v>53853</v>
       </c>
       <c r="D26" s="0">
-        <v>49317</v>
+        <v>52998</v>
       </c>
       <c r="E26" s="0">
-        <v>42852</v>
+        <v>46535</v>
       </c>
     </row>
     <row r="27">
@@ -1722,16 +1710,16 @@
         <v>30</v>
       </c>
       <c r="B27" s="0">
-        <v>55533</v>
+        <v>47990</v>
       </c>
       <c r="C27" s="0">
-        <v>55666</v>
+        <v>55380</v>
       </c>
       <c r="D27" s="0">
-        <v>54076</v>
+        <v>58141</v>
       </c>
       <c r="E27" s="0">
-        <v>43373</v>
+        <v>47137</v>
       </c>
     </row>
     <row r="28">
@@ -1739,16 +1727,16 @@
         <v>31</v>
       </c>
       <c r="B28" s="0">
-        <v>57372</v>
+        <v>49393</v>
       </c>
       <c r="C28" s="0">
-        <v>56329</v>
+        <v>56084</v>
       </c>
       <c r="D28" s="0">
-        <v>55281</v>
+        <v>59512</v>
       </c>
       <c r="E28" s="0">
-        <v>45556</v>
+        <v>49549</v>
       </c>
     </row>
     <row r="29">
@@ -1756,16 +1744,16 @@
         <v>32</v>
       </c>
       <c r="B29" s="0">
-        <v>60953</v>
+        <v>51719</v>
       </c>
       <c r="C29" s="0">
-        <v>61868</v>
+        <v>62125</v>
       </c>
       <c r="D29" s="0">
-        <v>56923</v>
+        <v>61858</v>
       </c>
       <c r="E29" s="0">
-        <v>48221</v>
+        <v>52263</v>
       </c>
     </row>
     <row r="30">
@@ -1773,16 +1761,16 @@
         <v>33</v>
       </c>
       <c r="B30" s="0">
-        <v>61566</v>
+        <v>53491</v>
       </c>
       <c r="C30" s="0">
-        <v>63148</v>
+        <v>62242</v>
       </c>
       <c r="D30" s="0">
-        <v>57601</v>
+        <v>62005</v>
       </c>
       <c r="E30" s="0">
-        <v>48444</v>
+        <v>53021</v>
       </c>
     </row>
     <row r="31">
@@ -1790,16 +1778,16 @@
         <v>34</v>
       </c>
       <c r="B31" s="0">
-        <v>64761</v>
+        <v>56501</v>
       </c>
       <c r="C31" s="0">
-        <v>67593</v>
+        <v>65772</v>
       </c>
       <c r="D31" s="0">
-        <v>60003</v>
+        <v>65187</v>
       </c>
       <c r="E31" s="0">
-        <v>54770</v>
+        <v>59667</v>
       </c>
     </row>
   </sheetData>
@@ -1807,7 +1795,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1817,30 +1805,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>953987</v>
+        <v>818063</v>
       </c>
       <c r="B2" s="0">
-        <v>953730</v>
+        <v>953926</v>
       </c>
       <c r="C2" s="0">
-        <v>884011</v>
+        <v>951615</v>
       </c>
       <c r="D2" s="0">
-        <v>748132</v>
+        <v>816256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
item statistic by age is added
</commit_message>
<xml_diff>
--- a/DataAgregation/age-clusters.xlsx
+++ b/DataAgregation/age-clusters.xlsx
@@ -9,13 +9,14 @@
     <sheet name="New Users" sheetId="25" r:id="rId35"/>
     <sheet name="Revenue" sheetId="26" r:id="rId36"/>
     <sheet name="MAU" sheetId="27" r:id="rId38"/>
+    <sheet name="Items Statistic" sheetId="28" r:id="rId39"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +133,369 @@
   </si>
   <si>
     <t>54-64</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>13-23</t>
+  </si>
+  <si>
+    <t>24-36</t>
+  </si>
+  <si>
+    <t>37-49</t>
+  </si>
+  <si>
+    <t>50-64</t>
+  </si>
+  <si>
+    <t>A Pony</t>
+  </si>
+  <si>
+    <t>Anarchist Cookbook</t>
+  </si>
+  <si>
+    <t>Best Friend</t>
+  </si>
+  <si>
+    <t>Black Hole</t>
+  </si>
+  <si>
+    <t>Blank Card</t>
+  </si>
+  <si>
+    <t>Blood Rights</t>
+  </si>
+  <si>
+    <t>Book of Revelations</t>
+  </si>
+  <si>
+    <t>Book of Secrets</t>
+  </si>
+  <si>
+    <t>Book of Shadows</t>
+  </si>
+  <si>
+    <t>Book of the Dead</t>
+  </si>
+  <si>
+    <t>Box of Friends</t>
+  </si>
+  <si>
+    <t>Box of Spiders</t>
+  </si>
+  <si>
+    <t>Breath of Life</t>
+  </si>
+  <si>
+    <t>Broken Shovel</t>
+  </si>
+  <si>
+    <t>Brown Nugget</t>
+  </si>
+  <si>
+    <t>Butter Bean</t>
+  </si>
+  <si>
+    <t>Clicker</t>
+  </si>
+  <si>
+    <t>Compost</t>
+  </si>
+  <si>
+    <t>Converter</t>
+  </si>
+  <si>
+    <t>Coupon</t>
+  </si>
+  <si>
+    <t>Crack the Sky</t>
+  </si>
+  <si>
+    <t>Crooked Penny</t>
+  </si>
+  <si>
+    <t>Crystal Ball</t>
+  </si>
+  <si>
+    <t>D Infinity</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D100</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D20</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>Dads Key</t>
+  </si>
+  <si>
+    <t>Dataminer</t>
+  </si>
+  <si>
+    <t>Dead Sea Scrolls</t>
+  </si>
+  <si>
+    <t>Deck of Cards</t>
+  </si>
+  <si>
+    <t>Delirious</t>
+  </si>
+  <si>
+    <t>Diplopia</t>
+  </si>
+  <si>
+    <t>Doctors Remote</t>
+  </si>
+  <si>
+    <t>Dull Razor</t>
+  </si>
+  <si>
+    <t>Edens Soul</t>
+  </si>
+  <si>
+    <t>Flush!</t>
+  </si>
+  <si>
+    <t>Forget Me Now</t>
+  </si>
+  <si>
+    <t>Friendly Ball</t>
+  </si>
+  <si>
+    <t>Glass Cannon</t>
+  </si>
+  <si>
+    <t>Glowing Hour Glass</t>
+  </si>
+  <si>
+    <t>Guppys Head</t>
+  </si>
+  <si>
+    <t>Guppys Paw</t>
+  </si>
+  <si>
+    <t>Head of Krampus</t>
+  </si>
+  <si>
+    <t>How to Jump</t>
+  </si>
+  <si>
+    <t>IV Bag</t>
+  </si>
+  <si>
+    <t>Jar of Flies</t>
+  </si>
+  <si>
+    <t>Kamikaze!</t>
+  </si>
+  <si>
+    <t>Kidney Bean</t>
+  </si>
+  <si>
+    <t>Lemon Mishap</t>
+  </si>
+  <si>
+    <t>Magic Fingers</t>
+  </si>
+  <si>
+    <t>Mama Mega!</t>
+  </si>
+  <si>
+    <t>Mega Bean</t>
+  </si>
+  <si>
+    <t>Mega Blast</t>
+  </si>
+  <si>
+    <t>Metronome</t>
+  </si>
+  <si>
+    <t>Mine Crafter</t>
+  </si>
+  <si>
+    <t>Moms Bottle of Pills</t>
+  </si>
+  <si>
+    <t>Moms Box</t>
+  </si>
+  <si>
+    <t>Moms Shovel</t>
+  </si>
+  <si>
+    <t>Monster Manual</t>
+  </si>
+  <si>
+    <t>Monstros Tooth</t>
+  </si>
+  <si>
+    <t>Moving Box</t>
+  </si>
+  <si>
+    <t>Mr. Boom</t>
+  </si>
+  <si>
+    <t>Mr. ME!</t>
+  </si>
+  <si>
+    <t>My Little Unicorn</t>
+  </si>
+  <si>
+    <t>Mystery Gift</t>
+  </si>
+  <si>
+    <t>Notched Axe</t>
+  </si>
+  <si>
+    <t>Pandoras Box</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>Placebo</t>
+  </si>
+  <si>
+    <t>Plan C</t>
+  </si>
+  <si>
+    <t>Portable Slot</t>
+  </si>
+  <si>
+    <t>Potato Peeler</t>
+  </si>
+  <si>
+    <t>Prayer Card</t>
+  </si>
+  <si>
+    <t>Razor Blade</t>
+  </si>
+  <si>
+    <t>Remote Detonator</t>
+  </si>
+  <si>
+    <t>Sacrificial Altar</t>
+  </si>
+  <si>
+    <t>Scissors</t>
+  </si>
+  <si>
+    <t>Sharp Straw</t>
+  </si>
+  <si>
+    <t>Shoop Da Whoop!</t>
+  </si>
+  <si>
+    <t>Sprinkler</t>
+  </si>
+  <si>
+    <t>Tammys Head</t>
+  </si>
+  <si>
+    <t>Tear Detonator</t>
+  </si>
+  <si>
+    <t>Telekinesis</t>
+  </si>
+  <si>
+    <t>Telepathy for Dummies</t>
+  </si>
+  <si>
+    <t>Teleport</t>
+  </si>
+  <si>
+    <t>Teleport 2.0</t>
+  </si>
+  <si>
+    <t>The Bean</t>
+  </si>
+  <si>
+    <t>The Book of Belial</t>
+  </si>
+  <si>
+    <t>The Book of Sin</t>
+  </si>
+  <si>
+    <t>The Boomerang</t>
+  </si>
+  <si>
+    <t>The Candle</t>
+  </si>
+  <si>
+    <t>The D6</t>
+  </si>
+  <si>
+    <t>The Gamekid</t>
+  </si>
+  <si>
+    <t>The Hourglass</t>
+  </si>
+  <si>
+    <t>The Jar</t>
+  </si>
+  <si>
+    <t>The Nail</t>
+  </si>
+  <si>
+    <t>The Necronomicon</t>
+  </si>
+  <si>
+    <t>The Pinking Shears</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>Unicorn Stump</t>
+  </si>
+  <si>
+    <t>Ventricle Razor</t>
+  </si>
+  <si>
+    <t>Void</t>
+  </si>
+  <si>
+    <t>Wait What?</t>
+  </si>
+  <si>
+    <t>We Need to Go Deeper!</t>
+  </si>
+  <si>
+    <t>White Pony</t>
+  </si>
+  <si>
+    <t>Wooden Nickel</t>
+  </si>
+  <si>
+    <t>Yum Heart</t>
   </si>
 </sst>
 </file>
@@ -1834,4 +2198,3703 @@
   </sheetData>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:J115"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="0">
+        <v>1705</v>
+      </c>
+      <c r="C3" s="0">
+        <v>2019</v>
+      </c>
+      <c r="D3" s="0">
+        <v>1966</v>
+      </c>
+      <c r="E3" s="0">
+        <v>2426</v>
+      </c>
+      <c r="F3" s="0">
+        <v>272800</v>
+      </c>
+      <c r="G3" s="0">
+        <v>323040</v>
+      </c>
+      <c r="H3" s="0">
+        <v>314560</v>
+      </c>
+      <c r="I3" s="0">
+        <v>388160</v>
+      </c>
+      <c r="J3" s="0">
+        <v>112514.1443322785</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="0">
+        <v>12041</v>
+      </c>
+      <c r="C4" s="0">
+        <v>13873</v>
+      </c>
+      <c r="D4" s="0">
+        <v>14002</v>
+      </c>
+      <c r="E4" s="0">
+        <v>16098</v>
+      </c>
+      <c r="F4" s="0">
+        <v>120410</v>
+      </c>
+      <c r="G4" s="0">
+        <v>138730</v>
+      </c>
+      <c r="H4" s="0">
+        <v>140020</v>
+      </c>
+      <c r="I4" s="0">
+        <v>160980</v>
+      </c>
+      <c r="J4" s="0">
+        <v>48533.122929872865</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="0">
+        <v>1341</v>
+      </c>
+      <c r="C5" s="0">
+        <v>1627</v>
+      </c>
+      <c r="D5" s="0">
+        <v>1492</v>
+      </c>
+      <c r="E5" s="0">
+        <v>1828</v>
+      </c>
+      <c r="F5" s="0">
+        <v>871650</v>
+      </c>
+      <c r="G5" s="0">
+        <v>1057550</v>
+      </c>
+      <c r="H5" s="0">
+        <v>969800</v>
+      </c>
+      <c r="I5" s="0">
+        <v>1188200</v>
+      </c>
+      <c r="J5" s="0">
+        <v>354134.76436482684</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="0">
+        <v>1347</v>
+      </c>
+      <c r="C6" s="0">
+        <v>1663</v>
+      </c>
+      <c r="D6" s="0">
+        <v>1597</v>
+      </c>
+      <c r="E6" s="0">
+        <v>1923</v>
+      </c>
+      <c r="F6" s="0">
+        <v>686970</v>
+      </c>
+      <c r="G6" s="0">
+        <v>848130</v>
+      </c>
+      <c r="H6" s="0">
+        <v>814470</v>
+      </c>
+      <c r="I6" s="0">
+        <v>980730</v>
+      </c>
+      <c r="J6" s="0">
+        <v>288551.9675669178</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="0">
+        <v>1535</v>
+      </c>
+      <c r="C7" s="0">
+        <v>1841</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1833</v>
+      </c>
+      <c r="E7" s="0">
+        <v>2101</v>
+      </c>
+      <c r="F7" s="0">
+        <v>368400</v>
+      </c>
+      <c r="G7" s="0">
+        <v>441840</v>
+      </c>
+      <c r="H7" s="0">
+        <v>439920</v>
+      </c>
+      <c r="I7" s="0">
+        <v>504240</v>
+      </c>
+      <c r="J7" s="0">
+        <v>152010.7703464421</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="0">
+        <v>2971</v>
+      </c>
+      <c r="C8" s="0">
+        <v>3508</v>
+      </c>
+      <c r="D8" s="0">
+        <v>3497</v>
+      </c>
+      <c r="E8" s="0">
+        <v>4096</v>
+      </c>
+      <c r="F8" s="0">
+        <v>297100</v>
+      </c>
+      <c r="G8" s="0">
+        <v>350800</v>
+      </c>
+      <c r="H8" s="0">
+        <v>349700</v>
+      </c>
+      <c r="I8" s="0">
+        <v>409600</v>
+      </c>
+      <c r="J8" s="0">
+        <v>121927.42312030277</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="0">
+        <v>2300</v>
+      </c>
+      <c r="C9" s="0">
+        <v>2642</v>
+      </c>
+      <c r="D9" s="0">
+        <v>2670</v>
+      </c>
+      <c r="E9" s="0">
+        <v>3080</v>
+      </c>
+      <c r="F9" s="0">
+        <v>276000</v>
+      </c>
+      <c r="G9" s="0">
+        <v>317040</v>
+      </c>
+      <c r="H9" s="0">
+        <v>320400</v>
+      </c>
+      <c r="I9" s="0">
+        <v>369600</v>
+      </c>
+      <c r="J9" s="0">
+        <v>111168.75329949813</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="0">
+        <v>1342</v>
+      </c>
+      <c r="C10" s="0">
+        <v>1555</v>
+      </c>
+      <c r="D10" s="0">
+        <v>1574</v>
+      </c>
+      <c r="E10" s="0">
+        <v>1772</v>
+      </c>
+      <c r="F10" s="0">
+        <v>885720</v>
+      </c>
+      <c r="G10" s="0">
+        <v>1026300</v>
+      </c>
+      <c r="H10" s="0">
+        <v>1038840</v>
+      </c>
+      <c r="I10" s="0">
+        <v>1169520</v>
+      </c>
+      <c r="J10" s="0">
+        <v>357007.142722546</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="0">
+        <v>1362</v>
+      </c>
+      <c r="C11" s="0">
+        <v>1587</v>
+      </c>
+      <c r="D11" s="0">
+        <v>1701</v>
+      </c>
+      <c r="E11" s="0">
+        <v>1864</v>
+      </c>
+      <c r="F11" s="0">
+        <v>681000</v>
+      </c>
+      <c r="G11" s="0">
+        <v>793500</v>
+      </c>
+      <c r="H11" s="0">
+        <v>850500</v>
+      </c>
+      <c r="I11" s="0">
+        <v>932000</v>
+      </c>
+      <c r="J11" s="0">
+        <v>282200.52097981924</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="0">
+        <v>12053</v>
+      </c>
+      <c r="C12" s="0">
+        <v>14129</v>
+      </c>
+      <c r="D12" s="0">
+        <v>14275</v>
+      </c>
+      <c r="E12" s="0">
+        <v>16331</v>
+      </c>
+      <c r="F12" s="0">
+        <v>241060</v>
+      </c>
+      <c r="G12" s="0">
+        <v>282580</v>
+      </c>
+      <c r="H12" s="0">
+        <v>285500</v>
+      </c>
+      <c r="I12" s="0">
+        <v>326620</v>
+      </c>
+      <c r="J12" s="0">
+        <v>98406.91923405693</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="0">
+        <v>2598</v>
+      </c>
+      <c r="C13" s="0">
+        <v>2980</v>
+      </c>
+      <c r="D13" s="0">
+        <v>2860</v>
+      </c>
+      <c r="E13" s="0">
+        <v>3513</v>
+      </c>
+      <c r="F13" s="0">
+        <v>285780</v>
+      </c>
+      <c r="G13" s="0">
+        <v>327800</v>
+      </c>
+      <c r="H13" s="0">
+        <v>314600</v>
+      </c>
+      <c r="I13" s="0">
+        <v>386430</v>
+      </c>
+      <c r="J13" s="0">
+        <v>113904.486794699</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="0">
+        <v>1546</v>
+      </c>
+      <c r="C14" s="0">
+        <v>1889</v>
+      </c>
+      <c r="D14" s="0">
+        <v>1730</v>
+      </c>
+      <c r="E14" s="0">
+        <v>2067</v>
+      </c>
+      <c r="F14" s="0">
+        <v>417420</v>
+      </c>
+      <c r="G14" s="0">
+        <v>510030</v>
+      </c>
+      <c r="H14" s="0">
+        <v>467100</v>
+      </c>
+      <c r="I14" s="0">
+        <v>558090</v>
+      </c>
+      <c r="J14" s="0">
+        <v>169186.66397046918</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="0">
+        <v>1361</v>
+      </c>
+      <c r="C15" s="0">
+        <v>1662</v>
+      </c>
+      <c r="D15" s="0">
+        <v>1612</v>
+      </c>
+      <c r="E15" s="0">
+        <v>1884</v>
+      </c>
+      <c r="F15" s="0">
+        <v>544400</v>
+      </c>
+      <c r="G15" s="0">
+        <v>664800</v>
+      </c>
+      <c r="H15" s="0">
+        <v>644800</v>
+      </c>
+      <c r="I15" s="0">
+        <v>753600</v>
+      </c>
+      <c r="J15" s="0">
+        <v>225937.15397536173</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="0">
+        <v>1402</v>
+      </c>
+      <c r="C16" s="0">
+        <v>1699</v>
+      </c>
+      <c r="D16" s="0">
+        <v>1630</v>
+      </c>
+      <c r="E16" s="0">
+        <v>1850</v>
+      </c>
+      <c r="F16" s="0">
+        <v>588840</v>
+      </c>
+      <c r="G16" s="0">
+        <v>713580</v>
+      </c>
+      <c r="H16" s="0">
+        <v>684600</v>
+      </c>
+      <c r="I16" s="0">
+        <v>777000</v>
+      </c>
+      <c r="J16" s="0">
+        <v>239487.55651262682</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="0">
+        <v>1412</v>
+      </c>
+      <c r="C17" s="0">
+        <v>1664</v>
+      </c>
+      <c r="D17" s="0">
+        <v>1589</v>
+      </c>
+      <c r="E17" s="0">
+        <v>1896</v>
+      </c>
+      <c r="F17" s="0">
+        <v>776600</v>
+      </c>
+      <c r="G17" s="0">
+        <v>915200</v>
+      </c>
+      <c r="H17" s="0">
+        <v>873950</v>
+      </c>
+      <c r="I17" s="0">
+        <v>1042800</v>
+      </c>
+      <c r="J17" s="0">
+        <v>312665.1656831164</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="0">
+        <v>8392</v>
+      </c>
+      <c r="C18" s="0">
+        <v>9923</v>
+      </c>
+      <c r="D18" s="0">
+        <v>9825</v>
+      </c>
+      <c r="E18" s="0">
+        <v>11356</v>
+      </c>
+      <c r="F18" s="0">
+        <v>503520</v>
+      </c>
+      <c r="G18" s="0">
+        <v>595380</v>
+      </c>
+      <c r="H18" s="0">
+        <v>589500</v>
+      </c>
+      <c r="I18" s="0">
+        <v>681360</v>
+      </c>
+      <c r="J18" s="0">
+        <v>205328.0556687648</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="0">
+        <v>1405</v>
+      </c>
+      <c r="C19" s="0">
+        <v>1759</v>
+      </c>
+      <c r="D19" s="0">
+        <v>1627</v>
+      </c>
+      <c r="E19" s="0">
+        <v>1906</v>
+      </c>
+      <c r="F19" s="0">
+        <v>505800</v>
+      </c>
+      <c r="G19" s="0">
+        <v>633240</v>
+      </c>
+      <c r="H19" s="0">
+        <v>585720</v>
+      </c>
+      <c r="I19" s="0">
+        <v>686160</v>
+      </c>
+      <c r="J19" s="0">
+        <v>208891.65779464325</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="0">
+        <v>1294</v>
+      </c>
+      <c r="C20" s="0">
+        <v>1551</v>
+      </c>
+      <c r="D20" s="0">
+        <v>1553</v>
+      </c>
+      <c r="E20" s="0">
+        <v>1796</v>
+      </c>
+      <c r="F20" s="0">
+        <v>815220</v>
+      </c>
+      <c r="G20" s="0">
+        <v>977130</v>
+      </c>
+      <c r="H20" s="0">
+        <v>978390</v>
+      </c>
+      <c r="I20" s="0">
+        <v>1131480</v>
+      </c>
+      <c r="J20" s="0">
+        <v>338106.7654517308</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="0">
+        <v>1296</v>
+      </c>
+      <c r="C21" s="0">
+        <v>1540</v>
+      </c>
+      <c r="D21" s="0">
+        <v>1556</v>
+      </c>
+      <c r="E21" s="0">
+        <v>1816</v>
+      </c>
+      <c r="F21" s="0">
+        <v>907200</v>
+      </c>
+      <c r="G21" s="0">
+        <v>1078000</v>
+      </c>
+      <c r="H21" s="0">
+        <v>1089200</v>
+      </c>
+      <c r="I21" s="0">
+        <v>1271200</v>
+      </c>
+      <c r="J21" s="0">
+        <v>376525.843196822</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="0">
+        <v>1484</v>
+      </c>
+      <c r="C22" s="0">
+        <v>1706</v>
+      </c>
+      <c r="D22" s="0">
+        <v>1730</v>
+      </c>
+      <c r="E22" s="0">
+        <v>2017</v>
+      </c>
+      <c r="F22" s="0">
+        <v>504560</v>
+      </c>
+      <c r="G22" s="0">
+        <v>580040</v>
+      </c>
+      <c r="H22" s="0">
+        <v>588200</v>
+      </c>
+      <c r="I22" s="0">
+        <v>685780</v>
+      </c>
+      <c r="J22" s="0">
+        <v>204355.20333072194</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="0">
+        <v>11994</v>
+      </c>
+      <c r="C23" s="0">
+        <v>14091</v>
+      </c>
+      <c r="D23" s="0">
+        <v>14116</v>
+      </c>
+      <c r="E23" s="0">
+        <v>16159</v>
+      </c>
+      <c r="F23" s="0">
+        <v>479760</v>
+      </c>
+      <c r="G23" s="0">
+        <v>563640</v>
+      </c>
+      <c r="H23" s="0">
+        <v>564640</v>
+      </c>
+      <c r="I23" s="0">
+        <v>646360</v>
+      </c>
+      <c r="J23" s="0">
+        <v>195331.32691974888</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="0">
+        <v>1650</v>
+      </c>
+      <c r="C24" s="0">
+        <v>1969</v>
+      </c>
+      <c r="D24" s="0">
+        <v>1871</v>
+      </c>
+      <c r="E24" s="0">
+        <v>2282</v>
+      </c>
+      <c r="F24" s="0">
+        <v>313500</v>
+      </c>
+      <c r="G24" s="0">
+        <v>374110</v>
+      </c>
+      <c r="H24" s="0">
+        <v>355490</v>
+      </c>
+      <c r="I24" s="0">
+        <v>433580</v>
+      </c>
+      <c r="J24" s="0">
+        <v>127947.73631183086</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="0">
+        <v>1349</v>
+      </c>
+      <c r="C25" s="0">
+        <v>1592</v>
+      </c>
+      <c r="D25" s="0">
+        <v>1589</v>
+      </c>
+      <c r="E25" s="0">
+        <v>1831</v>
+      </c>
+      <c r="F25" s="0">
+        <v>944300</v>
+      </c>
+      <c r="G25" s="0">
+        <v>1114400</v>
+      </c>
+      <c r="H25" s="0">
+        <v>1112300</v>
+      </c>
+      <c r="I25" s="0">
+        <v>1281700</v>
+      </c>
+      <c r="J25" s="0">
+        <v>385803.2657026764</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="0">
+        <v>1423</v>
+      </c>
+      <c r="C26" s="0">
+        <v>1640</v>
+      </c>
+      <c r="D26" s="0">
+        <v>1606</v>
+      </c>
+      <c r="E26" s="0">
+        <v>1798</v>
+      </c>
+      <c r="F26" s="0">
+        <v>868030</v>
+      </c>
+      <c r="G26" s="0">
+        <v>1000400</v>
+      </c>
+      <c r="H26" s="0">
+        <v>979660</v>
+      </c>
+      <c r="I26" s="0">
+        <v>1096780</v>
+      </c>
+      <c r="J26" s="0">
+        <v>341808.1661186817</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="0">
+        <v>1466</v>
+      </c>
+      <c r="C27" s="0">
+        <v>1644</v>
+      </c>
+      <c r="D27" s="0">
+        <v>1595</v>
+      </c>
+      <c r="E27" s="0">
+        <v>1986</v>
+      </c>
+      <c r="F27" s="0">
+        <v>498440</v>
+      </c>
+      <c r="G27" s="0">
+        <v>558960</v>
+      </c>
+      <c r="H27" s="0">
+        <v>542300</v>
+      </c>
+      <c r="I27" s="0">
+        <v>675240</v>
+      </c>
+      <c r="J27" s="0">
+        <v>197111.17761698063</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="0">
+        <v>1348</v>
+      </c>
+      <c r="C28" s="0">
+        <v>1590</v>
+      </c>
+      <c r="D28" s="0">
+        <v>1663</v>
+      </c>
+      <c r="E28" s="0">
+        <v>1901</v>
+      </c>
+      <c r="F28" s="0">
+        <v>768360</v>
+      </c>
+      <c r="G28" s="0">
+        <v>906300</v>
+      </c>
+      <c r="H28" s="0">
+        <v>947910</v>
+      </c>
+      <c r="I28" s="0">
+        <v>1083570</v>
+      </c>
+      <c r="J28" s="0">
+        <v>321115.0773021237</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="0">
+        <v>1476</v>
+      </c>
+      <c r="C29" s="0">
+        <v>1803</v>
+      </c>
+      <c r="D29" s="0">
+        <v>1763</v>
+      </c>
+      <c r="E29" s="0">
+        <v>2076</v>
+      </c>
+      <c r="F29" s="0">
+        <v>398520</v>
+      </c>
+      <c r="G29" s="0">
+        <v>486810</v>
+      </c>
+      <c r="H29" s="0">
+        <v>476010</v>
+      </c>
+      <c r="I29" s="0">
+        <v>560520</v>
+      </c>
+      <c r="J29" s="0">
+        <v>166517.91077295505</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="0">
+        <v>1711</v>
+      </c>
+      <c r="C30" s="0">
+        <v>2006</v>
+      </c>
+      <c r="D30" s="0">
+        <v>1959</v>
+      </c>
+      <c r="E30" s="0">
+        <v>2369</v>
+      </c>
+      <c r="F30" s="0">
+        <v>273760</v>
+      </c>
+      <c r="G30" s="0">
+        <v>320960</v>
+      </c>
+      <c r="H30" s="0">
+        <v>313440</v>
+      </c>
+      <c r="I30" s="0">
+        <v>379040</v>
+      </c>
+      <c r="J30" s="0">
+        <v>111531.10784352878</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="0">
+        <v>1365</v>
+      </c>
+      <c r="C31" s="0">
+        <v>1592</v>
+      </c>
+      <c r="D31" s="0">
+        <v>1513</v>
+      </c>
+      <c r="E31" s="0">
+        <v>1919</v>
+      </c>
+      <c r="F31" s="0">
+        <v>900900</v>
+      </c>
+      <c r="G31" s="0">
+        <v>1050720</v>
+      </c>
+      <c r="H31" s="0">
+        <v>998580</v>
+      </c>
+      <c r="I31" s="0">
+        <v>1266540</v>
+      </c>
+      <c r="J31" s="0">
+        <v>365359.4320323235</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="0">
+        <v>1441</v>
+      </c>
+      <c r="C32" s="0">
+        <v>1698</v>
+      </c>
+      <c r="D32" s="0">
+        <v>1685</v>
+      </c>
+      <c r="E32" s="0">
+        <v>2004</v>
+      </c>
+      <c r="F32" s="0">
+        <v>504350</v>
+      </c>
+      <c r="G32" s="0">
+        <v>594300</v>
+      </c>
+      <c r="H32" s="0">
+        <v>589750</v>
+      </c>
+      <c r="I32" s="0">
+        <v>701400</v>
+      </c>
+      <c r="J32" s="0">
+        <v>207063.72976994567</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="0">
+        <v>1703</v>
+      </c>
+      <c r="C33" s="0">
+        <v>2037</v>
+      </c>
+      <c r="D33" s="0">
+        <v>2081</v>
+      </c>
+      <c r="E33" s="0">
+        <v>2363</v>
+      </c>
+      <c r="F33" s="0">
+        <v>272480</v>
+      </c>
+      <c r="G33" s="0">
+        <v>325920</v>
+      </c>
+      <c r="H33" s="0">
+        <v>332960</v>
+      </c>
+      <c r="I33" s="0">
+        <v>378080</v>
+      </c>
+      <c r="J33" s="0">
+        <v>113455.50643510903</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="0">
+        <v>1611</v>
+      </c>
+      <c r="C34" s="0">
+        <v>1793</v>
+      </c>
+      <c r="D34" s="0">
+        <v>1818</v>
+      </c>
+      <c r="E34" s="0">
+        <v>2073</v>
+      </c>
+      <c r="F34" s="0">
+        <v>386640</v>
+      </c>
+      <c r="G34" s="0">
+        <v>430320</v>
+      </c>
+      <c r="H34" s="0">
+        <v>436320</v>
+      </c>
+      <c r="I34" s="0">
+        <v>497520</v>
+      </c>
+      <c r="J34" s="0">
+        <v>151697.1367459884</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="0">
+        <v>1413</v>
+      </c>
+      <c r="C35" s="0">
+        <v>1675</v>
+      </c>
+      <c r="D35" s="0">
+        <v>1679</v>
+      </c>
+      <c r="E35" s="0">
+        <v>1916</v>
+      </c>
+      <c r="F35" s="0">
+        <v>607590</v>
+      </c>
+      <c r="G35" s="0">
+        <v>720250</v>
+      </c>
+      <c r="H35" s="0">
+        <v>721970</v>
+      </c>
+      <c r="I35" s="0">
+        <v>823880</v>
+      </c>
+      <c r="J35" s="0">
+        <v>248991.56489937237</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="0">
+        <v>1364</v>
+      </c>
+      <c r="C36" s="0">
+        <v>1641</v>
+      </c>
+      <c r="D36" s="0">
+        <v>1587</v>
+      </c>
+      <c r="E36" s="0">
+        <v>1849</v>
+      </c>
+      <c r="F36" s="0">
+        <v>777480</v>
+      </c>
+      <c r="G36" s="0">
+        <v>935370</v>
+      </c>
+      <c r="H36" s="0">
+        <v>904590</v>
+      </c>
+      <c r="I36" s="0">
+        <v>1053930</v>
+      </c>
+      <c r="J36" s="0">
+        <v>318109.34523274266</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="0">
+        <v>1346</v>
+      </c>
+      <c r="C37" s="0">
+        <v>1537</v>
+      </c>
+      <c r="D37" s="0">
+        <v>1602</v>
+      </c>
+      <c r="E37" s="0">
+        <v>1844</v>
+      </c>
+      <c r="F37" s="0">
+        <v>726840</v>
+      </c>
+      <c r="G37" s="0">
+        <v>829980</v>
+      </c>
+      <c r="H37" s="0">
+        <v>865080</v>
+      </c>
+      <c r="I37" s="0">
+        <v>995760</v>
+      </c>
+      <c r="J37" s="0">
+        <v>296127.97947195574</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="0">
+        <v>1365</v>
+      </c>
+      <c r="C38" s="0">
+        <v>1640</v>
+      </c>
+      <c r="D38" s="0">
+        <v>1741</v>
+      </c>
+      <c r="E38" s="0">
+        <v>1929</v>
+      </c>
+      <c r="F38" s="0">
+        <v>641550</v>
+      </c>
+      <c r="G38" s="0">
+        <v>770800</v>
+      </c>
+      <c r="H38" s="0">
+        <v>818270</v>
+      </c>
+      <c r="I38" s="0">
+        <v>906630</v>
+      </c>
+      <c r="J38" s="0">
+        <v>271824.03898214444</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="0">
+        <v>1486</v>
+      </c>
+      <c r="C39" s="0">
+        <v>1766</v>
+      </c>
+      <c r="D39" s="0">
+        <v>1809</v>
+      </c>
+      <c r="E39" s="0">
+        <v>2135</v>
+      </c>
+      <c r="F39" s="0">
+        <v>401220</v>
+      </c>
+      <c r="G39" s="0">
+        <v>476820</v>
+      </c>
+      <c r="H39" s="0">
+        <v>488430</v>
+      </c>
+      <c r="I39" s="0">
+        <v>576450</v>
+      </c>
+      <c r="J39" s="0">
+        <v>168343.8603453572</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="0">
+        <v>1351</v>
+      </c>
+      <c r="C40" s="0">
+        <v>1615</v>
+      </c>
+      <c r="D40" s="0">
+        <v>1645</v>
+      </c>
+      <c r="E40" s="0">
+        <v>1841</v>
+      </c>
+      <c r="F40" s="0">
+        <v>634970</v>
+      </c>
+      <c r="G40" s="0">
+        <v>759050</v>
+      </c>
+      <c r="H40" s="0">
+        <v>773150</v>
+      </c>
+      <c r="I40" s="0">
+        <v>865270</v>
+      </c>
+      <c r="J40" s="0">
+        <v>262743.0734389629</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="0">
+        <v>1399</v>
+      </c>
+      <c r="C41" s="0">
+        <v>1662</v>
+      </c>
+      <c r="D41" s="0">
+        <v>1682</v>
+      </c>
+      <c r="E41" s="0">
+        <v>1959</v>
+      </c>
+      <c r="F41" s="0">
+        <v>475660</v>
+      </c>
+      <c r="G41" s="0">
+        <v>565080</v>
+      </c>
+      <c r="H41" s="0">
+        <v>571880</v>
+      </c>
+      <c r="I41" s="0">
+        <v>666060</v>
+      </c>
+      <c r="J41" s="0">
+        <v>197438.08671692197</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" s="0">
+        <v>1385</v>
+      </c>
+      <c r="C42" s="0">
+        <v>1734</v>
+      </c>
+      <c r="D42" s="0">
+        <v>1719</v>
+      </c>
+      <c r="E42" s="0">
+        <v>2002</v>
+      </c>
+      <c r="F42" s="0">
+        <v>457050</v>
+      </c>
+      <c r="G42" s="0">
+        <v>572220</v>
+      </c>
+      <c r="H42" s="0">
+        <v>567270</v>
+      </c>
+      <c r="I42" s="0">
+        <v>660660</v>
+      </c>
+      <c r="J42" s="0">
+        <v>195572.43759552372</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="0">
+        <v>1409</v>
+      </c>
+      <c r="C43" s="0">
+        <v>1577</v>
+      </c>
+      <c r="D43" s="0">
+        <v>1615</v>
+      </c>
+      <c r="E43" s="0">
+        <v>1874</v>
+      </c>
+      <c r="F43" s="0">
+        <v>704500</v>
+      </c>
+      <c r="G43" s="0">
+        <v>788500</v>
+      </c>
+      <c r="H43" s="0">
+        <v>807500</v>
+      </c>
+      <c r="I43" s="0">
+        <v>937000</v>
+      </c>
+      <c r="J43" s="0">
+        <v>280512.65137033025</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="0">
+        <v>12050</v>
+      </c>
+      <c r="C44" s="0">
+        <v>14039</v>
+      </c>
+      <c r="D44" s="0">
+        <v>14073</v>
+      </c>
+      <c r="E44" s="0">
+        <v>16215</v>
+      </c>
+      <c r="F44" s="0">
+        <v>120500</v>
+      </c>
+      <c r="G44" s="0">
+        <v>140390</v>
+      </c>
+      <c r="H44" s="0">
+        <v>140730</v>
+      </c>
+      <c r="I44" s="0">
+        <v>162150</v>
+      </c>
+      <c r="J44" s="0">
+        <v>48847.40392478979</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="0">
+        <v>1449</v>
+      </c>
+      <c r="C45" s="0">
+        <v>1621</v>
+      </c>
+      <c r="D45" s="0">
+        <v>1729</v>
+      </c>
+      <c r="E45" s="0">
+        <v>1913</v>
+      </c>
+      <c r="F45" s="0">
+        <v>463680</v>
+      </c>
+      <c r="G45" s="0">
+        <v>518720</v>
+      </c>
+      <c r="H45" s="0">
+        <v>553280</v>
+      </c>
+      <c r="I45" s="0">
+        <v>612160</v>
+      </c>
+      <c r="J45" s="0">
+        <v>186099.91453047429</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="0">
+        <v>1417</v>
+      </c>
+      <c r="C46" s="0">
+        <v>1665</v>
+      </c>
+      <c r="D46" s="0">
+        <v>1599</v>
+      </c>
+      <c r="E46" s="0">
+        <v>1882</v>
+      </c>
+      <c r="F46" s="0">
+        <v>580970</v>
+      </c>
+      <c r="G46" s="0">
+        <v>682650</v>
+      </c>
+      <c r="H46" s="0">
+        <v>655590</v>
+      </c>
+      <c r="I46" s="0">
+        <v>771620</v>
+      </c>
+      <c r="J46" s="0">
+        <v>233148.47554186502</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="0">
+        <v>1356</v>
+      </c>
+      <c r="C47" s="0">
+        <v>1633</v>
+      </c>
+      <c r="D47" s="0">
+        <v>1661</v>
+      </c>
+      <c r="E47" s="0">
+        <v>1869</v>
+      </c>
+      <c r="F47" s="0">
+        <v>623760</v>
+      </c>
+      <c r="G47" s="0">
+        <v>751180</v>
+      </c>
+      <c r="H47" s="0">
+        <v>764060</v>
+      </c>
+      <c r="I47" s="0">
+        <v>859740</v>
+      </c>
+      <c r="J47" s="0">
+        <v>259827.43993354874</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="0">
+        <v>1312</v>
+      </c>
+      <c r="C48" s="0">
+        <v>1533</v>
+      </c>
+      <c r="D48" s="0">
+        <v>1523</v>
+      </c>
+      <c r="E48" s="0">
+        <v>1808</v>
+      </c>
+      <c r="F48" s="0">
+        <v>892160</v>
+      </c>
+      <c r="G48" s="0">
+        <v>1042440</v>
+      </c>
+      <c r="H48" s="0">
+        <v>1035640</v>
+      </c>
+      <c r="I48" s="0">
+        <v>1229440</v>
+      </c>
+      <c r="J48" s="0">
+        <v>363880.6401889421</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="0">
+        <v>1424</v>
+      </c>
+      <c r="C49" s="0">
+        <v>1646</v>
+      </c>
+      <c r="D49" s="0">
+        <v>1617</v>
+      </c>
+      <c r="E49" s="0">
+        <v>1835</v>
+      </c>
+      <c r="F49" s="0">
+        <v>840160</v>
+      </c>
+      <c r="G49" s="0">
+        <v>971140</v>
+      </c>
+      <c r="H49" s="0">
+        <v>954030</v>
+      </c>
+      <c r="I49" s="0">
+        <v>1082650</v>
+      </c>
+      <c r="J49" s="0">
+        <v>333406.577565266</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="0">
+        <v>1396</v>
+      </c>
+      <c r="C50" s="0">
+        <v>1588</v>
+      </c>
+      <c r="D50" s="0">
+        <v>1601</v>
+      </c>
+      <c r="E50" s="0">
+        <v>1889</v>
+      </c>
+      <c r="F50" s="0">
+        <v>809680</v>
+      </c>
+      <c r="G50" s="0">
+        <v>921040</v>
+      </c>
+      <c r="H50" s="0">
+        <v>928580</v>
+      </c>
+      <c r="I50" s="0">
+        <v>1095620</v>
+      </c>
+      <c r="J50" s="0">
+        <v>325345.0547523477</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="0">
+        <v>2957</v>
+      </c>
+      <c r="C51" s="0">
+        <v>3532</v>
+      </c>
+      <c r="D51" s="0">
+        <v>3494</v>
+      </c>
+      <c r="E51" s="0">
+        <v>4211</v>
+      </c>
+      <c r="F51" s="0">
+        <v>59140</v>
+      </c>
+      <c r="G51" s="0">
+        <v>70640</v>
+      </c>
+      <c r="H51" s="0">
+        <v>69880</v>
+      </c>
+      <c r="I51" s="0">
+        <v>84220</v>
+      </c>
+      <c r="J51" s="0">
+        <v>24596.83983073827</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="0">
+        <v>1316</v>
+      </c>
+      <c r="C52" s="0">
+        <v>1504</v>
+      </c>
+      <c r="D52" s="0">
+        <v>1515</v>
+      </c>
+      <c r="E52" s="0">
+        <v>1752</v>
+      </c>
+      <c r="F52" s="0">
+        <v>868560</v>
+      </c>
+      <c r="G52" s="0">
+        <v>992640</v>
+      </c>
+      <c r="H52" s="0">
+        <v>999900</v>
+      </c>
+      <c r="I52" s="0">
+        <v>1156320</v>
+      </c>
+      <c r="J52" s="0">
+        <v>348090.6609435969</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="0">
+        <v>1301</v>
+      </c>
+      <c r="C53" s="0">
+        <v>1598</v>
+      </c>
+      <c r="D53" s="0">
+        <v>1539</v>
+      </c>
+      <c r="E53" s="0">
+        <v>1748</v>
+      </c>
+      <c r="F53" s="0">
+        <v>845650</v>
+      </c>
+      <c r="G53" s="0">
+        <v>1038700</v>
+      </c>
+      <c r="H53" s="0">
+        <v>1000350</v>
+      </c>
+      <c r="I53" s="0">
+        <v>1136200</v>
+      </c>
+      <c r="J53" s="0">
+        <v>348391.0410796082</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="0">
+        <v>1361</v>
+      </c>
+      <c r="C54" s="0">
+        <v>1614</v>
+      </c>
+      <c r="D54" s="0">
+        <v>1691</v>
+      </c>
+      <c r="E54" s="0">
+        <v>1866</v>
+      </c>
+      <c r="F54" s="0">
+        <v>585230</v>
+      </c>
+      <c r="G54" s="0">
+        <v>694020</v>
+      </c>
+      <c r="H54" s="0">
+        <v>727130</v>
+      </c>
+      <c r="I54" s="0">
+        <v>802380</v>
+      </c>
+      <c r="J54" s="0">
+        <v>243367.37345594072</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="0">
+        <v>1360</v>
+      </c>
+      <c r="C55" s="0">
+        <v>1648</v>
+      </c>
+      <c r="D55" s="0">
+        <v>1699</v>
+      </c>
+      <c r="E55" s="0">
+        <v>1951</v>
+      </c>
+      <c r="F55" s="0">
+        <v>503200</v>
+      </c>
+      <c r="G55" s="0">
+        <v>609760</v>
+      </c>
+      <c r="H55" s="0">
+        <v>628630</v>
+      </c>
+      <c r="I55" s="0">
+        <v>721870</v>
+      </c>
+      <c r="J55" s="0">
+        <v>213447.55458587132</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="0">
+        <v>3615</v>
+      </c>
+      <c r="C56" s="0">
+        <v>4251</v>
+      </c>
+      <c r="D56" s="0">
+        <v>4265</v>
+      </c>
+      <c r="E56" s="0">
+        <v>4945</v>
+      </c>
+      <c r="F56" s="0">
+        <v>325350</v>
+      </c>
+      <c r="G56" s="0">
+        <v>382590</v>
+      </c>
+      <c r="H56" s="0">
+        <v>383850</v>
+      </c>
+      <c r="I56" s="0">
+        <v>445050</v>
+      </c>
+      <c r="J56" s="0">
+        <v>133159.32260347833</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="0">
+        <v>1379</v>
+      </c>
+      <c r="C57" s="0">
+        <v>1626</v>
+      </c>
+      <c r="D57" s="0">
+        <v>1605</v>
+      </c>
+      <c r="E57" s="0">
+        <v>1854</v>
+      </c>
+      <c r="F57" s="0">
+        <v>537810</v>
+      </c>
+      <c r="G57" s="0">
+        <v>634140</v>
+      </c>
+      <c r="H57" s="0">
+        <v>625950</v>
+      </c>
+      <c r="I57" s="0">
+        <v>723060</v>
+      </c>
+      <c r="J57" s="0">
+        <v>218427.0695463138</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="0">
+        <v>1389</v>
+      </c>
+      <c r="C58" s="0">
+        <v>1640</v>
+      </c>
+      <c r="D58" s="0">
+        <v>1591</v>
+      </c>
+      <c r="E58" s="0">
+        <v>1902</v>
+      </c>
+      <c r="F58" s="0">
+        <v>708390</v>
+      </c>
+      <c r="G58" s="0">
+        <v>836400</v>
+      </c>
+      <c r="H58" s="0">
+        <v>811410</v>
+      </c>
+      <c r="I58" s="0">
+        <v>970020</v>
+      </c>
+      <c r="J58" s="0">
+        <v>288195.44939980615</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="0">
+        <v>1377</v>
+      </c>
+      <c r="C59" s="0">
+        <v>1675</v>
+      </c>
+      <c r="D59" s="0">
+        <v>1669</v>
+      </c>
+      <c r="E59" s="0">
+        <v>1898</v>
+      </c>
+      <c r="F59" s="0">
+        <v>743580</v>
+      </c>
+      <c r="G59" s="0">
+        <v>904500</v>
+      </c>
+      <c r="H59" s="0">
+        <v>901260</v>
+      </c>
+      <c r="I59" s="0">
+        <v>1024920</v>
+      </c>
+      <c r="J59" s="0">
+        <v>309693.9122626296</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B60" s="0">
+        <v>1376</v>
+      </c>
+      <c r="C60" s="0">
+        <v>1657</v>
+      </c>
+      <c r="D60" s="0">
+        <v>1617</v>
+      </c>
+      <c r="E60" s="0">
+        <v>1841</v>
+      </c>
+      <c r="F60" s="0">
+        <v>715520</v>
+      </c>
+      <c r="G60" s="0">
+        <v>861640</v>
+      </c>
+      <c r="H60" s="0">
+        <v>840840</v>
+      </c>
+      <c r="I60" s="0">
+        <v>957320</v>
+      </c>
+      <c r="J60" s="0">
+        <v>292450.39054636523</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="0">
+        <v>1422</v>
+      </c>
+      <c r="C61" s="0">
+        <v>1777</v>
+      </c>
+      <c r="D61" s="0">
+        <v>1750</v>
+      </c>
+      <c r="E61" s="0">
+        <v>2010</v>
+      </c>
+      <c r="F61" s="0">
+        <v>412380</v>
+      </c>
+      <c r="G61" s="0">
+        <v>515330</v>
+      </c>
+      <c r="H61" s="0">
+        <v>507500</v>
+      </c>
+      <c r="I61" s="0">
+        <v>582900</v>
+      </c>
+      <c r="J61" s="0">
+        <v>174859.61596184573</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="0">
+        <v>1385</v>
+      </c>
+      <c r="C62" s="0">
+        <v>1771</v>
+      </c>
+      <c r="D62" s="0">
+        <v>1709</v>
+      </c>
+      <c r="E62" s="0">
+        <v>1952</v>
+      </c>
+      <c r="F62" s="0">
+        <v>470900</v>
+      </c>
+      <c r="G62" s="0">
+        <v>602140</v>
+      </c>
+      <c r="H62" s="0">
+        <v>581060</v>
+      </c>
+      <c r="I62" s="0">
+        <v>663680</v>
+      </c>
+      <c r="J62" s="0">
+        <v>200821.59459782593</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="0">
+        <v>1735</v>
+      </c>
+      <c r="C63" s="0">
+        <v>1943</v>
+      </c>
+      <c r="D63" s="0">
+        <v>2099</v>
+      </c>
+      <c r="E63" s="0">
+        <v>2267</v>
+      </c>
+      <c r="F63" s="0">
+        <v>294950</v>
+      </c>
+      <c r="G63" s="0">
+        <v>330310</v>
+      </c>
+      <c r="H63" s="0">
+        <v>356830</v>
+      </c>
+      <c r="I63" s="0">
+        <v>385390</v>
+      </c>
+      <c r="J63" s="0">
+        <v>118485.71953093051</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" s="0">
+        <v>1410</v>
+      </c>
+      <c r="C64" s="0">
+        <v>1670</v>
+      </c>
+      <c r="D64" s="0">
+        <v>1617</v>
+      </c>
+      <c r="E64" s="0">
+        <v>1878</v>
+      </c>
+      <c r="F64" s="0">
+        <v>747300</v>
+      </c>
+      <c r="G64" s="0">
+        <v>885100</v>
+      </c>
+      <c r="H64" s="0">
+        <v>857010</v>
+      </c>
+      <c r="I64" s="0">
+        <v>995340</v>
+      </c>
+      <c r="J64" s="0">
+        <v>301933.0461902694</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B65" s="0">
+        <v>1372</v>
+      </c>
+      <c r="C65" s="0">
+        <v>1524</v>
+      </c>
+      <c r="D65" s="0">
+        <v>1621</v>
+      </c>
+      <c r="E65" s="0">
+        <v>1770</v>
+      </c>
+      <c r="F65" s="0">
+        <v>644840</v>
+      </c>
+      <c r="G65" s="0">
+        <v>716280</v>
+      </c>
+      <c r="H65" s="0">
+        <v>761870</v>
+      </c>
+      <c r="I65" s="0">
+        <v>831900</v>
+      </c>
+      <c r="J65" s="0">
+        <v>256026.21572733883</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="0">
+        <v>1352</v>
+      </c>
+      <c r="C66" s="0">
+        <v>1673</v>
+      </c>
+      <c r="D66" s="0">
+        <v>1521</v>
+      </c>
+      <c r="E66" s="0">
+        <v>1942</v>
+      </c>
+      <c r="F66" s="0">
+        <v>608400</v>
+      </c>
+      <c r="G66" s="0">
+        <v>752850</v>
+      </c>
+      <c r="H66" s="0">
+        <v>684450</v>
+      </c>
+      <c r="I66" s="0">
+        <v>873900</v>
+      </c>
+      <c r="J66" s="0">
+        <v>252971.6865074702</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B67" s="0">
+        <v>1434</v>
+      </c>
+      <c r="C67" s="0">
+        <v>1587</v>
+      </c>
+      <c r="D67" s="0">
+        <v>1675</v>
+      </c>
+      <c r="E67" s="0">
+        <v>1911</v>
+      </c>
+      <c r="F67" s="0">
+        <v>616620</v>
+      </c>
+      <c r="G67" s="0">
+        <v>682410</v>
+      </c>
+      <c r="H67" s="0">
+        <v>720250</v>
+      </c>
+      <c r="I67" s="0">
+        <v>821730</v>
+      </c>
+      <c r="J67" s="0">
+        <v>246158.62238998822</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" s="0">
+        <v>11893</v>
+      </c>
+      <c r="C68" s="0">
+        <v>14164</v>
+      </c>
+      <c r="D68" s="0">
+        <v>14030</v>
+      </c>
+      <c r="E68" s="0">
+        <v>16273</v>
+      </c>
+      <c r="F68" s="0">
+        <v>118930</v>
+      </c>
+      <c r="G68" s="0">
+        <v>141640</v>
+      </c>
+      <c r="H68" s="0">
+        <v>140300</v>
+      </c>
+      <c r="I68" s="0">
+        <v>162730</v>
+      </c>
+      <c r="J68" s="0">
+        <v>48832.86090533279</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B69" s="0">
+        <v>2089</v>
+      </c>
+      <c r="C69" s="0">
+        <v>2439</v>
+      </c>
+      <c r="D69" s="0">
+        <v>2372</v>
+      </c>
+      <c r="E69" s="0">
+        <v>2821</v>
+      </c>
+      <c r="F69" s="0">
+        <v>271570</v>
+      </c>
+      <c r="G69" s="0">
+        <v>317070</v>
+      </c>
+      <c r="H69" s="0">
+        <v>308360</v>
+      </c>
+      <c r="I69" s="0">
+        <v>366730</v>
+      </c>
+      <c r="J69" s="0">
+        <v>109496.81055626296</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B70" s="0">
+        <v>1363</v>
+      </c>
+      <c r="C70" s="0">
+        <v>1581</v>
+      </c>
+      <c r="D70" s="0">
+        <v>1667</v>
+      </c>
+      <c r="E70" s="0">
+        <v>1888</v>
+      </c>
+      <c r="F70" s="0">
+        <v>667870</v>
+      </c>
+      <c r="G70" s="0">
+        <v>774690</v>
+      </c>
+      <c r="H70" s="0">
+        <v>816830</v>
+      </c>
+      <c r="I70" s="0">
+        <v>925120</v>
+      </c>
+      <c r="J70" s="0">
+        <v>275926.48573683086</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B71" s="0">
+        <v>1289</v>
+      </c>
+      <c r="C71" s="0">
+        <v>1537</v>
+      </c>
+      <c r="D71" s="0">
+        <v>1561</v>
+      </c>
+      <c r="E71" s="0">
+        <v>1808</v>
+      </c>
+      <c r="F71" s="0">
+        <v>876520</v>
+      </c>
+      <c r="G71" s="0">
+        <v>1045160</v>
+      </c>
+      <c r="H71" s="0">
+        <v>1061480</v>
+      </c>
+      <c r="I71" s="0">
+        <v>1229440</v>
+      </c>
+      <c r="J71" s="0">
+        <v>364992.1354745487</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" s="0">
+        <v>1404</v>
+      </c>
+      <c r="C72" s="0">
+        <v>1679</v>
+      </c>
+      <c r="D72" s="0">
+        <v>1631</v>
+      </c>
+      <c r="E72" s="0">
+        <v>1911</v>
+      </c>
+      <c r="F72" s="0">
+        <v>533520</v>
+      </c>
+      <c r="G72" s="0">
+        <v>638020</v>
+      </c>
+      <c r="H72" s="0">
+        <v>619780</v>
+      </c>
+      <c r="I72" s="0">
+        <v>726180</v>
+      </c>
+      <c r="J72" s="0">
+        <v>218131.52507445824</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="0">
+        <v>1801</v>
+      </c>
+      <c r="C73" s="0">
+        <v>2140</v>
+      </c>
+      <c r="D73" s="0">
+        <v>2225</v>
+      </c>
+      <c r="E73" s="0">
+        <v>2555</v>
+      </c>
+      <c r="F73" s="0">
+        <v>270150</v>
+      </c>
+      <c r="G73" s="0">
+        <v>321000</v>
+      </c>
+      <c r="H73" s="0">
+        <v>333750</v>
+      </c>
+      <c r="I73" s="0">
+        <v>383250</v>
+      </c>
+      <c r="J73" s="0">
+        <v>113344.23769676976</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" s="0">
+        <v>1524</v>
+      </c>
+      <c r="C74" s="0">
+        <v>1836</v>
+      </c>
+      <c r="D74" s="0">
+        <v>1862</v>
+      </c>
+      <c r="E74" s="0">
+        <v>2237</v>
+      </c>
+      <c r="F74" s="0">
+        <v>335280</v>
+      </c>
+      <c r="G74" s="0">
+        <v>403920</v>
+      </c>
+      <c r="H74" s="0">
+        <v>409640</v>
+      </c>
+      <c r="I74" s="0">
+        <v>492140</v>
+      </c>
+      <c r="J74" s="0">
+        <v>142180.40066970815</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="0">
+        <v>8405</v>
+      </c>
+      <c r="C75" s="0">
+        <v>10009</v>
+      </c>
+      <c r="D75" s="0">
+        <v>9963</v>
+      </c>
+      <c r="E75" s="0">
+        <v>11207</v>
+      </c>
+      <c r="F75" s="0">
+        <v>504300</v>
+      </c>
+      <c r="G75" s="0">
+        <v>600540</v>
+      </c>
+      <c r="H75" s="0">
+        <v>597780</v>
+      </c>
+      <c r="I75" s="0">
+        <v>672420</v>
+      </c>
+      <c r="J75" s="0">
+        <v>205784.9520538077</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" s="0">
+        <v>1467</v>
+      </c>
+      <c r="C76" s="0">
+        <v>1613</v>
+      </c>
+      <c r="D76" s="0">
+        <v>1749</v>
+      </c>
+      <c r="E76" s="0">
+        <v>2064</v>
+      </c>
+      <c r="F76" s="0">
+        <v>440100</v>
+      </c>
+      <c r="G76" s="0">
+        <v>483900</v>
+      </c>
+      <c r="H76" s="0">
+        <v>524700</v>
+      </c>
+      <c r="I76" s="0">
+        <v>619200</v>
+      </c>
+      <c r="J76" s="0">
+        <v>179173.86775519195</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="0">
+        <v>1341</v>
+      </c>
+      <c r="C77" s="0">
+        <v>1573</v>
+      </c>
+      <c r="D77" s="0">
+        <v>1561</v>
+      </c>
+      <c r="E77" s="0">
+        <v>1882</v>
+      </c>
+      <c r="F77" s="0">
+        <v>590040</v>
+      </c>
+      <c r="G77" s="0">
+        <v>692120</v>
+      </c>
+      <c r="H77" s="0">
+        <v>686840</v>
+      </c>
+      <c r="I77" s="0">
+        <v>828080</v>
+      </c>
+      <c r="J77" s="0">
+        <v>242352.6013198244</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" s="0">
+        <v>1359</v>
+      </c>
+      <c r="C78" s="0">
+        <v>1552</v>
+      </c>
+      <c r="D78" s="0">
+        <v>1601</v>
+      </c>
+      <c r="E78" s="0">
+        <v>1807</v>
+      </c>
+      <c r="F78" s="0">
+        <v>747450</v>
+      </c>
+      <c r="G78" s="0">
+        <v>853600</v>
+      </c>
+      <c r="H78" s="0">
+        <v>880550</v>
+      </c>
+      <c r="I78" s="0">
+        <v>993850</v>
+      </c>
+      <c r="J78" s="0">
+        <v>301132.2725059961</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79" s="0">
+        <v>1367</v>
+      </c>
+      <c r="C79" s="0">
+        <v>1621</v>
+      </c>
+      <c r="D79" s="0">
+        <v>1607</v>
+      </c>
+      <c r="E79" s="0">
+        <v>1931</v>
+      </c>
+      <c r="F79" s="0">
+        <v>560470</v>
+      </c>
+      <c r="G79" s="0">
+        <v>664610</v>
+      </c>
+      <c r="H79" s="0">
+        <v>658870</v>
+      </c>
+      <c r="I79" s="0">
+        <v>791710</v>
+      </c>
+      <c r="J79" s="0">
+        <v>231834.67959989177</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80" s="0">
+        <v>1872</v>
+      </c>
+      <c r="C80" s="0">
+        <v>2108</v>
+      </c>
+      <c r="D80" s="0">
+        <v>2149</v>
+      </c>
+      <c r="E80" s="0">
+        <v>2503</v>
+      </c>
+      <c r="F80" s="0">
+        <v>280800</v>
+      </c>
+      <c r="G80" s="0">
+        <v>316200</v>
+      </c>
+      <c r="H80" s="0">
+        <v>322350</v>
+      </c>
+      <c r="I80" s="0">
+        <v>375450</v>
+      </c>
+      <c r="J80" s="0">
+        <v>112189.33086084864</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="0">
+        <v>2061</v>
+      </c>
+      <c r="C81" s="0">
+        <v>2497</v>
+      </c>
+      <c r="D81" s="0">
+        <v>2413</v>
+      </c>
+      <c r="E81" s="0">
+        <v>2910</v>
+      </c>
+      <c r="F81" s="0">
+        <v>267930</v>
+      </c>
+      <c r="G81" s="0">
+        <v>324610</v>
+      </c>
+      <c r="H81" s="0">
+        <v>313690</v>
+      </c>
+      <c r="I81" s="0">
+        <v>378300</v>
+      </c>
+      <c r="J81" s="0">
+        <v>111298.32703453372</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" s="0">
+        <v>1670</v>
+      </c>
+      <c r="C82" s="0">
+        <v>1924</v>
+      </c>
+      <c r="D82" s="0">
+        <v>1984</v>
+      </c>
+      <c r="E82" s="0">
+        <v>2317</v>
+      </c>
+      <c r="F82" s="0">
+        <v>283900</v>
+      </c>
+      <c r="G82" s="0">
+        <v>327080</v>
+      </c>
+      <c r="H82" s="0">
+        <v>337280</v>
+      </c>
+      <c r="I82" s="0">
+        <v>393890</v>
+      </c>
+      <c r="J82" s="0">
+        <v>116289.17306419516</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B83" s="0">
+        <v>1657</v>
+      </c>
+      <c r="C83" s="0">
+        <v>2016</v>
+      </c>
+      <c r="D83" s="0">
+        <v>1991</v>
+      </c>
+      <c r="E83" s="0">
+        <v>2327</v>
+      </c>
+      <c r="F83" s="0">
+        <v>281690</v>
+      </c>
+      <c r="G83" s="0">
+        <v>342720</v>
+      </c>
+      <c r="H83" s="0">
+        <v>338470</v>
+      </c>
+      <c r="I83" s="0">
+        <v>395590</v>
+      </c>
+      <c r="J83" s="0">
+        <v>117703.16340049806</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" s="0">
+        <v>1359</v>
+      </c>
+      <c r="C84" s="0">
+        <v>1600</v>
+      </c>
+      <c r="D84" s="0">
+        <v>1628</v>
+      </c>
+      <c r="E84" s="0">
+        <v>1842</v>
+      </c>
+      <c r="F84" s="0">
+        <v>815400</v>
+      </c>
+      <c r="G84" s="0">
+        <v>960000</v>
+      </c>
+      <c r="H84" s="0">
+        <v>976800</v>
+      </c>
+      <c r="I84" s="0">
+        <v>1105200</v>
+      </c>
+      <c r="J84" s="0">
+        <v>334224.3424737674</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B85" s="0">
+        <v>1506</v>
+      </c>
+      <c r="C85" s="0">
+        <v>1818</v>
+      </c>
+      <c r="D85" s="0">
+        <v>1755</v>
+      </c>
+      <c r="E85" s="0">
+        <v>2042</v>
+      </c>
+      <c r="F85" s="0">
+        <v>451800</v>
+      </c>
+      <c r="G85" s="0">
+        <v>545400</v>
+      </c>
+      <c r="H85" s="0">
+        <v>526500</v>
+      </c>
+      <c r="I85" s="0">
+        <v>612600</v>
+      </c>
+      <c r="J85" s="0">
+        <v>185097.67757822404</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B86" s="0">
+        <v>1340</v>
+      </c>
+      <c r="C86" s="0">
+        <v>1565</v>
+      </c>
+      <c r="D86" s="0">
+        <v>1563</v>
+      </c>
+      <c r="E86" s="0">
+        <v>1803</v>
+      </c>
+      <c r="F86" s="0">
+        <v>938000</v>
+      </c>
+      <c r="G86" s="0">
+        <v>1095500</v>
+      </c>
+      <c r="H86" s="0">
+        <v>1094100</v>
+      </c>
+      <c r="I86" s="0">
+        <v>1262100</v>
+      </c>
+      <c r="J86" s="0">
+        <v>380346.4905227156</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B87" s="0">
+        <v>11965</v>
+      </c>
+      <c r="C87" s="0">
+        <v>14188</v>
+      </c>
+      <c r="D87" s="0">
+        <v>14207</v>
+      </c>
+      <c r="E87" s="0">
+        <v>16343</v>
+      </c>
+      <c r="F87" s="0">
+        <v>358950</v>
+      </c>
+      <c r="G87" s="0">
+        <v>425640</v>
+      </c>
+      <c r="H87" s="0">
+        <v>426210</v>
+      </c>
+      <c r="I87" s="0">
+        <v>490290</v>
+      </c>
+      <c r="J87" s="0">
+        <v>147390.89345209702</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B88" s="0">
+        <v>2239</v>
+      </c>
+      <c r="C88" s="0">
+        <v>2713</v>
+      </c>
+      <c r="D88" s="0">
+        <v>2597</v>
+      </c>
+      <c r="E88" s="0">
+        <v>3113</v>
+      </c>
+      <c r="F88" s="0">
+        <v>223900</v>
+      </c>
+      <c r="G88" s="0">
+        <v>271300</v>
+      </c>
+      <c r="H88" s="0">
+        <v>259700</v>
+      </c>
+      <c r="I88" s="0">
+        <v>311300</v>
+      </c>
+      <c r="J88" s="0">
+        <v>92380.38401664968</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B89" s="0">
+        <v>1835</v>
+      </c>
+      <c r="C89" s="0">
+        <v>2129</v>
+      </c>
+      <c r="D89" s="0">
+        <v>2110</v>
+      </c>
+      <c r="E89" s="0">
+        <v>2453</v>
+      </c>
+      <c r="F89" s="0">
+        <v>275250</v>
+      </c>
+      <c r="G89" s="0">
+        <v>319350</v>
+      </c>
+      <c r="H89" s="0">
+        <v>316500</v>
+      </c>
+      <c r="I89" s="0">
+        <v>367950</v>
+      </c>
+      <c r="J89" s="0">
+        <v>110821.77715617362</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B90" s="0">
+        <v>1418</v>
+      </c>
+      <c r="C90" s="0">
+        <v>1591</v>
+      </c>
+      <c r="D90" s="0">
+        <v>1667</v>
+      </c>
+      <c r="E90" s="0">
+        <v>1892</v>
+      </c>
+      <c r="F90" s="0">
+        <v>567200</v>
+      </c>
+      <c r="G90" s="0">
+        <v>636400</v>
+      </c>
+      <c r="H90" s="0">
+        <v>666800</v>
+      </c>
+      <c r="I90" s="0">
+        <v>756800</v>
+      </c>
+      <c r="J90" s="0">
+        <v>227631.30625017599</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B91" s="0">
+        <v>1317</v>
+      </c>
+      <c r="C91" s="0">
+        <v>1624</v>
+      </c>
+      <c r="D91" s="0">
+        <v>1566</v>
+      </c>
+      <c r="E91" s="0">
+        <v>1782</v>
+      </c>
+      <c r="F91" s="0">
+        <v>816540</v>
+      </c>
+      <c r="G91" s="0">
+        <v>1006880</v>
+      </c>
+      <c r="H91" s="0">
+        <v>970920</v>
+      </c>
+      <c r="I91" s="0">
+        <v>1104840</v>
+      </c>
+      <c r="J91" s="0">
+        <v>337842.83450086205</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B92" s="0">
+        <v>1416</v>
+      </c>
+      <c r="C92" s="0">
+        <v>1680</v>
+      </c>
+      <c r="D92" s="0">
+        <v>1616</v>
+      </c>
+      <c r="E92" s="0">
+        <v>1932</v>
+      </c>
+      <c r="F92" s="0">
+        <v>509760</v>
+      </c>
+      <c r="G92" s="0">
+        <v>604800</v>
+      </c>
+      <c r="H92" s="0">
+        <v>581760</v>
+      </c>
+      <c r="I92" s="0">
+        <v>695520</v>
+      </c>
+      <c r="J92" s="0">
+        <v>207241.57564861514</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B93" s="0">
+        <v>12075</v>
+      </c>
+      <c r="C93" s="0">
+        <v>14107</v>
+      </c>
+      <c r="D93" s="0">
+        <v>14131</v>
+      </c>
+      <c r="E93" s="0">
+        <v>16115</v>
+      </c>
+      <c r="F93" s="0">
+        <v>120750</v>
+      </c>
+      <c r="G93" s="0">
+        <v>141070</v>
+      </c>
+      <c r="H93" s="0">
+        <v>141310</v>
+      </c>
+      <c r="I93" s="0">
+        <v>161150</v>
+      </c>
+      <c r="J93" s="0">
+        <v>48891.699438122254</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B94" s="0">
+        <v>11986</v>
+      </c>
+      <c r="C94" s="0">
+        <v>14139</v>
+      </c>
+      <c r="D94" s="0">
+        <v>13958</v>
+      </c>
+      <c r="E94" s="0">
+        <v>16392</v>
+      </c>
+      <c r="F94" s="0">
+        <v>119860</v>
+      </c>
+      <c r="G94" s="0">
+        <v>141390</v>
+      </c>
+      <c r="H94" s="0">
+        <v>139580</v>
+      </c>
+      <c r="I94" s="0">
+        <v>163920</v>
+      </c>
+      <c r="J94" s="0">
+        <v>48932.32712227184</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B95" s="0">
+        <v>3009</v>
+      </c>
+      <c r="C95" s="0">
+        <v>3409</v>
+      </c>
+      <c r="D95" s="0">
+        <v>3480</v>
+      </c>
+      <c r="E95" s="0">
+        <v>4067</v>
+      </c>
+      <c r="F95" s="0">
+        <v>300900</v>
+      </c>
+      <c r="G95" s="0">
+        <v>340900</v>
+      </c>
+      <c r="H95" s="0">
+        <v>348000</v>
+      </c>
+      <c r="I95" s="0">
+        <v>406700</v>
+      </c>
+      <c r="J95" s="0">
+        <v>120999.47074515004</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B96" s="0">
+        <v>1335</v>
+      </c>
+      <c r="C96" s="0">
+        <v>1634</v>
+      </c>
+      <c r="D96" s="0">
+        <v>1620</v>
+      </c>
+      <c r="E96" s="0">
+        <v>1875</v>
+      </c>
+      <c r="F96" s="0">
+        <v>841050</v>
+      </c>
+      <c r="G96" s="0">
+        <v>1029420</v>
+      </c>
+      <c r="H96" s="0">
+        <v>1020600</v>
+      </c>
+      <c r="I96" s="0">
+        <v>1181250</v>
+      </c>
+      <c r="J96" s="0">
+        <v>352847.4822785258</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="0">
+        <v>3659</v>
+      </c>
+      <c r="C97" s="0">
+        <v>4206</v>
+      </c>
+      <c r="D97" s="0">
+        <v>4258</v>
+      </c>
+      <c r="E97" s="0">
+        <v>4985</v>
+      </c>
+      <c r="F97" s="0">
+        <v>329310</v>
+      </c>
+      <c r="G97" s="0">
+        <v>378540</v>
+      </c>
+      <c r="H97" s="0">
+        <v>383220</v>
+      </c>
+      <c r="I97" s="0">
+        <v>448650</v>
+      </c>
+      <c r="J97" s="0">
+        <v>133409.03547984964</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B98" s="0">
+        <v>1306</v>
+      </c>
+      <c r="C98" s="0">
+        <v>1556</v>
+      </c>
+      <c r="D98" s="0">
+        <v>1519</v>
+      </c>
+      <c r="E98" s="0">
+        <v>1775</v>
+      </c>
+      <c r="F98" s="0">
+        <v>888080</v>
+      </c>
+      <c r="G98" s="0">
+        <v>1058080</v>
+      </c>
+      <c r="H98" s="0">
+        <v>1032920</v>
+      </c>
+      <c r="I98" s="0">
+        <v>1207000</v>
+      </c>
+      <c r="J98" s="0">
+        <v>362704.8765550878</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B99" s="0">
+        <v>1755</v>
+      </c>
+      <c r="C99" s="0">
+        <v>2029</v>
+      </c>
+      <c r="D99" s="0">
+        <v>2090</v>
+      </c>
+      <c r="E99" s="0">
+        <v>2385</v>
+      </c>
+      <c r="F99" s="0">
+        <v>280800</v>
+      </c>
+      <c r="G99" s="0">
+        <v>324640</v>
+      </c>
+      <c r="H99" s="0">
+        <v>334400</v>
+      </c>
+      <c r="I99" s="0">
+        <v>381600</v>
+      </c>
+      <c r="J99" s="0">
+        <v>114496.57483503706</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B100" s="0">
+        <v>1366</v>
+      </c>
+      <c r="C100" s="0">
+        <v>1669</v>
+      </c>
+      <c r="D100" s="0">
+        <v>1649</v>
+      </c>
+      <c r="E100" s="0">
+        <v>1910</v>
+      </c>
+      <c r="F100" s="0">
+        <v>532740</v>
+      </c>
+      <c r="G100" s="0">
+        <v>650910</v>
+      </c>
+      <c r="H100" s="0">
+        <v>643110</v>
+      </c>
+      <c r="I100" s="0">
+        <v>744900</v>
+      </c>
+      <c r="J100" s="0">
+        <v>222819.0502155986</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B101" s="0">
+        <v>1405</v>
+      </c>
+      <c r="C101" s="0">
+        <v>1611</v>
+      </c>
+      <c r="D101" s="0">
+        <v>1612</v>
+      </c>
+      <c r="E101" s="0">
+        <v>1787</v>
+      </c>
+      <c r="F101" s="0">
+        <v>702500</v>
+      </c>
+      <c r="G101" s="0">
+        <v>805500</v>
+      </c>
+      <c r="H101" s="0">
+        <v>806000</v>
+      </c>
+      <c r="I101" s="0">
+        <v>893500</v>
+      </c>
+      <c r="J101" s="0">
+        <v>277909.3026291239</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B102" s="0">
+        <v>4745</v>
+      </c>
+      <c r="C102" s="0">
+        <v>5654</v>
+      </c>
+      <c r="D102" s="0">
+        <v>5655</v>
+      </c>
+      <c r="E102" s="0">
+        <v>6712</v>
+      </c>
+      <c r="F102" s="0">
+        <v>379600</v>
+      </c>
+      <c r="G102" s="0">
+        <v>452320</v>
+      </c>
+      <c r="H102" s="0">
+        <v>452400</v>
+      </c>
+      <c r="I102" s="0">
+        <v>536960</v>
+      </c>
+      <c r="J102" s="0">
+        <v>157803.97514393576</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B103" s="0">
+        <v>1434</v>
+      </c>
+      <c r="C103" s="0">
+        <v>1615</v>
+      </c>
+      <c r="D103" s="0">
+        <v>1645</v>
+      </c>
+      <c r="E103" s="0">
+        <v>1806</v>
+      </c>
+      <c r="F103" s="0">
+        <v>731340</v>
+      </c>
+      <c r="G103" s="0">
+        <v>823650</v>
+      </c>
+      <c r="H103" s="0">
+        <v>838950</v>
+      </c>
+      <c r="I103" s="0">
+        <v>921060</v>
+      </c>
+      <c r="J103" s="0">
+        <v>287236.3516698953</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B104" s="0">
+        <v>1406</v>
+      </c>
+      <c r="C104" s="0">
+        <v>1550</v>
+      </c>
+      <c r="D104" s="0">
+        <v>1550</v>
+      </c>
+      <c r="E104" s="0">
+        <v>1801</v>
+      </c>
+      <c r="F104" s="0">
+        <v>759240</v>
+      </c>
+      <c r="G104" s="0">
+        <v>837000</v>
+      </c>
+      <c r="H104" s="0">
+        <v>837000</v>
+      </c>
+      <c r="I104" s="0">
+        <v>972540</v>
+      </c>
+      <c r="J104" s="0">
+        <v>295090.6574020676</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B105" s="0">
+        <v>1396</v>
+      </c>
+      <c r="C105" s="0">
+        <v>1681</v>
+      </c>
+      <c r="D105" s="0">
+        <v>1661</v>
+      </c>
+      <c r="E105" s="0">
+        <v>1864</v>
+      </c>
+      <c r="F105" s="0">
+        <v>628200</v>
+      </c>
+      <c r="G105" s="0">
+        <v>756450</v>
+      </c>
+      <c r="H105" s="0">
+        <v>747450</v>
+      </c>
+      <c r="I105" s="0">
+        <v>838800</v>
+      </c>
+      <c r="J105" s="0">
+        <v>257415.4770859671</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B106" s="0">
+        <v>6402</v>
+      </c>
+      <c r="C106" s="0">
+        <v>7526</v>
+      </c>
+      <c r="D106" s="0">
+        <v>7485</v>
+      </c>
+      <c r="E106" s="0">
+        <v>8625</v>
+      </c>
+      <c r="F106" s="0">
+        <v>448140</v>
+      </c>
+      <c r="G106" s="0">
+        <v>526820</v>
+      </c>
+      <c r="H106" s="0">
+        <v>523950</v>
+      </c>
+      <c r="I106" s="0">
+        <v>603750</v>
+      </c>
+      <c r="J106" s="0">
+        <v>182184.2849620059</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B107" s="0">
+        <v>1508</v>
+      </c>
+      <c r="C107" s="0">
+        <v>1848</v>
+      </c>
+      <c r="D107" s="0">
+        <v>1835</v>
+      </c>
+      <c r="E107" s="0">
+        <v>2152</v>
+      </c>
+      <c r="F107" s="0">
+        <v>407160</v>
+      </c>
+      <c r="G107" s="0">
+        <v>498960</v>
+      </c>
+      <c r="H107" s="0">
+        <v>495450</v>
+      </c>
+      <c r="I107" s="0">
+        <v>581040</v>
+      </c>
+      <c r="J107" s="0">
+        <v>171783.3855028275</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B108" s="0">
+        <v>1311</v>
+      </c>
+      <c r="C108" s="0">
+        <v>1644</v>
+      </c>
+      <c r="D108" s="0">
+        <v>1657</v>
+      </c>
+      <c r="E108" s="0">
+        <v>1841</v>
+      </c>
+      <c r="F108" s="0">
+        <v>786600</v>
+      </c>
+      <c r="G108" s="0">
+        <v>986400</v>
+      </c>
+      <c r="H108" s="0">
+        <v>994200</v>
+      </c>
+      <c r="I108" s="0">
+        <v>1104600</v>
+      </c>
+      <c r="J108" s="0">
+        <v>335471.7423073774</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B109" s="0">
+        <v>1494</v>
+      </c>
+      <c r="C109" s="0">
+        <v>1677</v>
+      </c>
+      <c r="D109" s="0">
+        <v>1822</v>
+      </c>
+      <c r="E109" s="0">
+        <v>2058</v>
+      </c>
+      <c r="F109" s="0">
+        <v>433260</v>
+      </c>
+      <c r="G109" s="0">
+        <v>486330</v>
+      </c>
+      <c r="H109" s="0">
+        <v>528380</v>
+      </c>
+      <c r="I109" s="0">
+        <v>596820</v>
+      </c>
+      <c r="J109" s="0">
+        <v>177174.2124124577</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B110" s="0">
+        <v>1329</v>
+      </c>
+      <c r="C110" s="0">
+        <v>1620</v>
+      </c>
+      <c r="D110" s="0">
+        <v>1625</v>
+      </c>
+      <c r="E110" s="0">
+        <v>1907</v>
+      </c>
+      <c r="F110" s="0">
+        <v>744240</v>
+      </c>
+      <c r="G110" s="0">
+        <v>907200</v>
+      </c>
+      <c r="H110" s="0">
+        <v>910000</v>
+      </c>
+      <c r="I110" s="0">
+        <v>1067920</v>
+      </c>
+      <c r="J110" s="0">
+        <v>314462.31904466223</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B111" s="0">
+        <v>1322</v>
+      </c>
+      <c r="C111" s="0">
+        <v>1595</v>
+      </c>
+      <c r="D111" s="0">
+        <v>1442</v>
+      </c>
+      <c r="E111" s="0">
+        <v>1772</v>
+      </c>
+      <c r="F111" s="0">
+        <v>898960</v>
+      </c>
+      <c r="G111" s="0">
+        <v>1084600</v>
+      </c>
+      <c r="H111" s="0">
+        <v>980560</v>
+      </c>
+      <c r="I111" s="0">
+        <v>1204960</v>
+      </c>
+      <c r="J111" s="0">
+        <v>361229.9407013793</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B112" s="0">
+        <v>1338</v>
+      </c>
+      <c r="C112" s="0">
+        <v>1611</v>
+      </c>
+      <c r="D112" s="0">
+        <v>1713</v>
+      </c>
+      <c r="E112" s="0">
+        <v>2008</v>
+      </c>
+      <c r="F112" s="0">
+        <v>508440</v>
+      </c>
+      <c r="G112" s="0">
+        <v>612180</v>
+      </c>
+      <c r="H112" s="0">
+        <v>650940</v>
+      </c>
+      <c r="I112" s="0">
+        <v>763040</v>
+      </c>
+      <c r="J112" s="0">
+        <v>219613.35697954564</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B113" s="0">
+        <v>1401</v>
+      </c>
+      <c r="C113" s="0">
+        <v>1598</v>
+      </c>
+      <c r="D113" s="0">
+        <v>1640</v>
+      </c>
+      <c r="E113" s="0">
+        <v>1869</v>
+      </c>
+      <c r="F113" s="0">
+        <v>812580</v>
+      </c>
+      <c r="G113" s="0">
+        <v>926840</v>
+      </c>
+      <c r="H113" s="0">
+        <v>951200</v>
+      </c>
+      <c r="I113" s="0">
+        <v>1084020</v>
+      </c>
+      <c r="J113" s="0">
+        <v>327052.7545693647</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B114" s="0">
+        <v>2555</v>
+      </c>
+      <c r="C114" s="0">
+        <v>2953</v>
+      </c>
+      <c r="D114" s="0">
+        <v>3026</v>
+      </c>
+      <c r="E114" s="0">
+        <v>3529</v>
+      </c>
+      <c r="F114" s="0">
+        <v>281050</v>
+      </c>
+      <c r="G114" s="0">
+        <v>324830</v>
+      </c>
+      <c r="H114" s="0">
+        <v>332860</v>
+      </c>
+      <c r="I114" s="0">
+        <v>388190</v>
+      </c>
+      <c r="J114" s="0">
+        <v>114971.10401061297</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B115" s="0">
+        <v>1479</v>
+      </c>
+      <c r="C115" s="0">
+        <v>1595</v>
+      </c>
+      <c r="D115" s="0">
+        <v>1641</v>
+      </c>
+      <c r="E115" s="0">
+        <v>2013</v>
+      </c>
+      <c r="F115" s="0">
+        <v>517650</v>
+      </c>
+      <c r="G115" s="0">
+        <v>558250</v>
+      </c>
+      <c r="H115" s="0">
+        <v>574350</v>
+      </c>
+      <c r="I115" s="0">
+        <v>704550</v>
+      </c>
+      <c r="J115" s="0">
+        <v>204030.53563442337</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:J2"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>